<commit_message>
Added Week 04 WBS and refined deliverables
</commit_message>
<xml_diff>
--- a/planning/ProjectPlan_Week03_A4.xlsx
+++ b/planning/ProjectPlan_Week03_A4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\BuiBui's Space\Learning Material\Degree Y3S1\AI Project Management\AIPM-A4\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6608AA00-593A-408A-AEF2-F90F4202AA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41541F97-2140-400C-949E-7894721F090A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectPlan_Week03" sheetId="1" r:id="rId1"/>
@@ -814,7 +814,7 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.796875" customWidth="1"/>
     <col min="2" max="2" width="24.796875" customWidth="1"/>
@@ -831,7 +831,7 @@
     <col min="16" max="18" width="32.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -887,7 +887,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -940,7 +940,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -993,7 +993,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1330,13 +1330,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.796875" customWidth="1"/>
     <col min="2" max="2" width="40.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -1372,11 +1372,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D958F6EF-C817-4061-953A-93C56B660F33}">
   <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:R17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="T39" sqref="T39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="8.8984375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2291,7 +2294,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52D2370C-56E8-4562-AB81-A656A9A155F3}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add estimated cost on the week 04 plan
</commit_message>
<xml_diff>
--- a/planning/ProjectPlan_Week03_A4.xlsx
+++ b/planning/ProjectPlan_Week03_A4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\BuiBui's Space\Learning Material\Degree Y3S1\AI Project Management\AIPM-A4\planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alici\Downloads\BAIX Y3S1\AI Project Management\AIPM-A4\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80111646-AC8B-4F26-AF91-190C2B9FE09C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A525BB97-8189-4F32-A53F-D969FD125A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectPlan_Week03" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="168">
   <si>
     <t>Task ID</t>
   </si>
@@ -602,6 +602,9 @@
 Quantity/Hours: 6 hrs_x000D_
 _x000D_
 Description: Test task creation, chat responses, and calendar sync for reliability</t>
+  </si>
+  <si>
+    <t>Estimated Cost (RM)</t>
   </si>
 </sst>
 </file>
@@ -984,24 +987,24 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="32.796875" customWidth="1"/>
-    <col min="2" max="2" width="24.796875" customWidth="1"/>
-    <col min="3" max="3" width="18.796875" customWidth="1"/>
-    <col min="4" max="4" width="14.796875" customWidth="1"/>
-    <col min="5" max="5" width="18.796875" customWidth="1"/>
-    <col min="6" max="6" width="24.796875" customWidth="1"/>
-    <col min="7" max="7" width="18.796875" customWidth="1"/>
-    <col min="8" max="10" width="11.796875" customWidth="1"/>
-    <col min="11" max="12" width="8.796875" customWidth="1"/>
-    <col min="13" max="13" width="11.796875" customWidth="1"/>
-    <col min="14" max="14" width="18.796875" customWidth="1"/>
-    <col min="15" max="15" width="8.796875" customWidth="1"/>
-    <col min="16" max="18" width="32.796875" customWidth="1"/>
+    <col min="1" max="1" width="32.78515625" customWidth="1"/>
+    <col min="2" max="2" width="24.78515625" customWidth="1"/>
+    <col min="3" max="3" width="18.78515625" customWidth="1"/>
+    <col min="4" max="4" width="14.78515625" customWidth="1"/>
+    <col min="5" max="5" width="18.78515625" customWidth="1"/>
+    <col min="6" max="6" width="24.78515625" customWidth="1"/>
+    <col min="7" max="7" width="18.78515625" customWidth="1"/>
+    <col min="8" max="10" width="11.78515625" customWidth="1"/>
+    <col min="11" max="12" width="8.78515625" customWidth="1"/>
+    <col min="13" max="13" width="11.78515625" customWidth="1"/>
+    <col min="14" max="14" width="18.78515625" customWidth="1"/>
+    <col min="15" max="15" width="8.78515625" customWidth="1"/>
+    <col min="16" max="18" width="32.78515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1057,7 +1060,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1110,7 +1113,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -1163,7 +1166,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -1216,7 +1219,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -1269,7 +1272,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -1322,7 +1325,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1375,7 +1378,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -1428,7 +1431,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1500,13 +1503,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.796875" customWidth="1"/>
-    <col min="2" max="2" width="40.796875" customWidth="1"/>
+    <col min="1" max="1" width="20.78515625" customWidth="1"/>
+    <col min="2" max="2" width="40.78515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -1514,7 +1517,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -1522,7 +1525,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -1540,19 +1543,35 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D958F6EF-C817-4061-953A-93C56B660F33}">
-  <dimension ref="A1:R17"/>
+  <dimension ref="A1:S17"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="T39" sqref="T39"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.8984375" customWidth="1"/>
+    <col min="1" max="1" width="8.640625" customWidth="1"/>
+    <col min="2" max="2" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.640625" customWidth="1"/>
+    <col min="6" max="6" width="37.0703125" customWidth="1"/>
+    <col min="7" max="7" width="15.92578125" customWidth="1"/>
+    <col min="8" max="8" width="11.78515625" customWidth="1"/>
+    <col min="9" max="10" width="11.2109375" customWidth="1"/>
+    <col min="11" max="11" width="10.92578125" customWidth="1"/>
+    <col min="12" max="12" width="7.0703125" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" customWidth="1"/>
+    <col min="14" max="14" width="13.0703125" customWidth="1"/>
+    <col min="15" max="15" width="22.85546875" customWidth="1"/>
+    <col min="16" max="16" width="13.35546875" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" customWidth="1"/>
+    <col min="18" max="18" width="11.640625" customWidth="1"/>
+    <col min="19" max="19" width="17.35546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1607,8 +1626,11 @@
       <c r="R1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -1660,8 +1682,11 @@
       <c r="Q2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -1713,8 +1738,11 @@
       <c r="Q3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -1766,8 +1794,11 @@
       <c r="Q4" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>82</v>
       </c>
@@ -1819,8 +1850,11 @@
       <c r="Q5" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S5">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>85</v>
       </c>
@@ -1872,8 +1906,11 @@
       <c r="Q6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S6">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>89</v>
       </c>
@@ -1925,8 +1962,11 @@
       <c r="Q7" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S7">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>92</v>
       </c>
@@ -1978,8 +2018,11 @@
       <c r="Q8" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S8">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>95</v>
       </c>
@@ -2031,8 +2074,11 @@
       <c r="Q9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S9">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>98</v>
       </c>
@@ -2084,8 +2130,11 @@
       <c r="Q10" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S10">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>102</v>
       </c>
@@ -2137,8 +2186,11 @@
       <c r="Q11" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S11">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>106</v>
       </c>
@@ -2190,8 +2242,11 @@
       <c r="Q12" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>109</v>
       </c>
@@ -2243,8 +2298,11 @@
       <c r="Q13" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>113</v>
       </c>
@@ -2296,8 +2354,11 @@
       <c r="Q14" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>117</v>
       </c>
@@ -2349,8 +2410,11 @@
       <c r="Q15" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S15">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>121</v>
       </c>
@@ -2402,8 +2466,11 @@
       <c r="Q16" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>125</v>
       </c>
@@ -2454,6 +2521,9 @@
       </c>
       <c r="Q17" t="s">
         <v>29</v>
+      </c>
+      <c r="S17">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2469,9 +2539,9 @@
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -2479,7 +2549,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -2487,7 +2557,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -2504,28 +2574,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F9767C5-ACC3-43E2-91BE-ABA7B317FA15}">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection sqref="A1:R11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="32.796875" customWidth="1"/>
-    <col min="2" max="2" width="24.796875" customWidth="1"/>
-    <col min="3" max="3" width="18.796875" customWidth="1"/>
-    <col min="4" max="4" width="14.796875" customWidth="1"/>
-    <col min="5" max="5" width="18.796875" customWidth="1"/>
-    <col min="6" max="6" width="24.796875" customWidth="1"/>
-    <col min="7" max="7" width="18.796875" customWidth="1"/>
-    <col min="8" max="10" width="11.796875" customWidth="1"/>
-    <col min="11" max="12" width="8.796875" customWidth="1"/>
-    <col min="13" max="13" width="11.796875" customWidth="1"/>
-    <col min="14" max="14" width="18.796875" customWidth="1"/>
-    <col min="15" max="15" width="8.796875" customWidth="1"/>
-    <col min="16" max="18" width="32.796875" customWidth="1"/>
+    <col min="1" max="18" width="8.640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2581,7 +2639,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>131</v>
       </c>
@@ -2637,7 +2695,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>133</v>
       </c>
@@ -2693,7 +2751,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>134</v>
       </c>
@@ -2749,7 +2807,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>136</v>
       </c>
@@ -2805,7 +2863,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>138</v>
       </c>
@@ -2861,7 +2919,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>139</v>
       </c>
@@ -2917,7 +2975,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>141</v>
       </c>
@@ -2973,7 +3031,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>158</v>
       </c>
@@ -3029,7 +3087,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>161</v>
       </c>
@@ -3085,7 +3143,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>164</v>
       </c>
@@ -3150,17 +3208,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA098234-68F1-46DD-8335-E6F59E6E06D7}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.796875" customWidth="1"/>
-    <col min="2" max="2" width="40.796875" customWidth="1"/>
+    <col min="1" max="1" width="20.78515625" customWidth="1"/>
+    <col min="2" max="2" width="40.78515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -3168,7 +3226,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -3176,7 +3234,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>68</v>
       </c>

</xml_diff>